<commit_message>
very minor edits to o&m costs and prioritization doc
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240814.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240814.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763CC0AE-94B3-4F9D-A594-A8B770FC31AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A9E0A6-5CAE-4B08-9FAE-B7EC4D67C6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1643,7 +1643,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1701,18 +1701,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2500,10 +2488,10 @@
   <dimension ref="A1:AG64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF62" sqref="AF62"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -8855,7 +8843,7 @@
         <v>19205</v>
       </c>
       <c r="T56" s="19">
-        <f t="shared" ref="R56:Y56" si="43">SUMIFS(T$2:T$52,$D$2:$D$52,$Q56,T$2:T$52,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="T56:X56" si="43">SUMIFS(T$2:T$52,$D$2:$D$52,$Q56,T$2:T$52,"&lt;&gt;#N/A")</f>
         <v>172400</v>
       </c>
       <c r="U56" s="19">

</xml_diff>

<commit_message>
updated during today's prioritiziation mtg
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240814.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240814.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A9E0A6-5CAE-4B08-9FAE-B7EC4D67C6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAF61F2-4153-4723-9891-0FB5CABD4CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2487,7 +2487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9373,7 +9373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A2C2A-A63B-4175-BFD5-FBED9F37A1FC}">
   <dimension ref="A1:AW47"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AW1"/>
     </sheetView>
   </sheetViews>

</xml_diff>